<commit_message>
Unit 2301 and 2302 fixes
</commit_message>
<xml_diff>
--- a/book2/2301/file/2301-naloga6.xlsx
+++ b/book2/2301/file/2301-naloga6.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB\rin2-dev\2301\file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB\rin2\book2\2301\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -61,7 +61,7 @@
     <t>Drnulja</t>
   </si>
   <si>
-    <t>0203952B00123</t>
+    <t>0203952500137</t>
   </si>
   <si>
     <t>Andraž</t>
@@ -70,7 +70,7 @@
     <t>Slamorezec</t>
   </si>
   <si>
-    <t>1308959B00124</t>
+    <t>1308959500124</t>
   </si>
   <si>
     <t>Pavla</t>
@@ -79,7 +79,7 @@
     <t>Zaropotaj</t>
   </si>
   <si>
-    <t>2203962B10234</t>
+    <t>2203962505231</t>
   </si>
   <si>
     <t>Jurček</t>
@@ -88,7 +88,7 @@
     <t>Griža</t>
   </si>
   <si>
-    <t>1809955B00218</t>
+    <t>1809955500218</t>
   </si>
   <si>
     <t>Bošte</t>
@@ -97,7 +97,7 @@
     <t>Krevs</t>
   </si>
   <si>
-    <t>2710963B00314</t>
+    <t>2710963500313</t>
   </si>
   <si>
     <t>Petra</t>
@@ -106,7 +106,7 @@
     <t>Strama</t>
   </si>
   <si>
-    <t>3107964B10278</t>
+    <t>3107964505276</t>
   </si>
   <si>
     <t>Marko</t>
@@ -115,7 +115,7 @@
     <t>Črmaž</t>
   </si>
   <si>
-    <t>2811000B00011</t>
+    <t>2811000500017</t>
   </si>
   <si>
     <t>Špela</t>
@@ -124,7 +124,7 @@
     <t>Kišovar</t>
   </si>
   <si>
-    <t>1402001B10456</t>
+    <t>1402001505453</t>
   </si>
 </sst>
 </file>
@@ -168,9 +168,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Navadno" xfId="0" builtinId="0"/>
@@ -488,7 +489,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -532,7 +533,7 @@
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -543,7 +544,7 @@
       <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -554,7 +555,7 @@
       <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -565,7 +566,7 @@
       <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -576,7 +577,7 @@
       <c r="B6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -587,7 +588,7 @@
       <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -598,7 +599,7 @@
       <c r="B8" t="s">
         <v>27</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -609,11 +610,14 @@
       <c r="B9" t="s">
         <v>30</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="C2:C9" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>